<commit_message>
add sheetname to constructor
</commit_message>
<xml_diff>
--- a/test/xlsx/Reestr_subektov_predprinimatelskoy_deyatelnostiosushchestvlyayushchih_dobychu_nefti_1.xlsx
+++ b/test/xlsx/Reestr_subektov_predprinimatelskoy_deyatelnostiosushchestvlyayushchih_dobychu_nefti_1.xlsx
@@ -487,7 +487,7 @@
         <v/>
       </c>
       <c r="C10" t="str" xml:space="preserve">
-        <v xml:space="preserve">
+        <v xml:space="preserve">_x000d_
 </v>
       </c>
     </row>
@@ -609,7 +609,7 @@
         <v>ООО «Северо-Варьеганское»</v>
       </c>
       <c r="C21" t="str" xml:space="preserve">
-        <v xml:space="preserve">Ханты-Мансийский автономный округ-Югра, 
+        <v xml:space="preserve">Ханты-Мансийский автономный округ-Югра, _x000d_
 г. Нижневартовск, Кузоваткина ул., 14</v>
       </c>
     </row>
@@ -621,7 +621,7 @@
         <v>АО «ННП»</v>
       </c>
       <c r="C22" t="str" xml:space="preserve">
-        <v xml:space="preserve">Ханты-Мансийский автономный округ-Югра, 
+        <v xml:space="preserve">Ханты-Мансийский автономный округ-Югра, _x000d_
 г. Нижневартовск, ул. Ленина, д. 17, корп. П</v>
       </c>
     </row>
@@ -655,7 +655,7 @@
         <v>АО «Корпорация Югранефть»</v>
       </c>
       <c r="C25" t="str" xml:space="preserve">
-        <v xml:space="preserve">Ханты-Мансийский автономный округ-Югра,
+        <v xml:space="preserve">Ханты-Мансийский автономный округ-Югра,_x000d_
  г. Нижневартовск,ул. Кузоватнкина, д. 14</v>
       </c>
     </row>
@@ -678,7 +678,7 @@
         <v>АО «Самотлорнефтегаз»</v>
       </c>
       <c r="C27" t="str" xml:space="preserve">
-        <v xml:space="preserve">Ханты-Мансийский автономный округ-Югра,
+        <v xml:space="preserve">Ханты-Мансийский автономный округ-Югра,_x000d_
  г. Нижневартовск, ул. Ленина, д. 4</v>
       </c>
     </row>
@@ -690,8 +690,8 @@
         <v>АО «РН-Няганьнефтегаз»</v>
       </c>
       <c r="C28" t="str" xml:space="preserve">
-        <v xml:space="preserve">Ханты-Мансийский автономный округ-Югра, г. Нягань, 
-ул. Сибирская, д. 10, корп. 1
+        <v xml:space="preserve">Ханты-Мансийский автономный округ-Югра, г. Нягань, _x000d_
+ул. Сибирская, д. 10, корп. 1_x000d_
 </v>
       </c>
     </row>
@@ -711,13 +711,13 @@
         <v>1.28</v>
       </c>
       <c r="B30" t="str" xml:space="preserve">
-        <v xml:space="preserve">ООО «Тагульское»
+        <v xml:space="preserve">ООО «Тагульское»_x000d_
 </v>
       </c>
       <c r="C30" t="str" xml:space="preserve">
-        <v xml:space="preserve">Красноярский край, 
-г. Красноярск, 
-ул. 78 Добровольческой бригады, д. 15
+        <v xml:space="preserve">Красноярский край, _x000d_
+г. Красноярск, _x000d_
+ул. 78 Добровольческой бригады, д. 15_x000d_
 </v>
       </c>
     </row>
@@ -784,7 +784,7 @@
         <v>ООО «ЛУКОЙЛ-АИК»</v>
       </c>
       <c r="C36" t="str" xml:space="preserve">
-        <v xml:space="preserve">Ханты-Мансийский автономный округ - Югра, город Когалым,улица Мира, дом 23, корпус А
+        <v xml:space="preserve">Ханты-Мансийский автономный округ - Югра, город Когалым,улица Мира, дом 23, корпус А_x000d_
 </v>
       </c>
     </row>
@@ -1093,7 +1093,7 @@
         <v>ООО «Меретояханефтегаз»</v>
       </c>
       <c r="C64" t="str" xml:space="preserve">
-        <v xml:space="preserve">Ямало-Ненецкий автономный округ, г. Надым, ул. Комсомольская, д.16, кв. 36
+        <v xml:space="preserve">Ямало-Ненецкий автономный округ, г. Надым, ул. Комсомольская, д.16, кв. 36_x000d_
 </v>
       </c>
     </row>
@@ -2026,9 +2026,9 @@
         <v>20.1</v>
       </c>
       <c r="B149" t="str" xml:space="preserve">
-        <v xml:space="preserve">Акционерное общество 
-«Нефтяная компания Дулисьма»
-(АО «НК Дулисьма»)
+        <v xml:space="preserve">Акционерное общество _x000d_
+«Нефтяная компания Дулисьма»_x000d_
+(АО «НК Дулисьма»)_x000d_
 </v>
       </c>
       <c r="C149" t="str">
@@ -2065,7 +2065,7 @@
         <v>АО «ИНК-Запад»</v>
       </c>
       <c r="C152" t="str" xml:space="preserve">
-        <v xml:space="preserve">Иркутская область, г. Иркутск, пр-т Большой Литейный, д. 4
+        <v xml:space="preserve">Иркутская область, г. Иркутск, пр-т Большой Литейный, д. 4_x000d_
 </v>
       </c>
     </row>
@@ -2341,8 +2341,8 @@
         <v>Акционерное общество «Геолого-разведочный исследовательский центр» (АО «ГРИЦ»)</v>
       </c>
       <c r="C177" t="str" xml:space="preserve">
-        <v xml:space="preserve">Республика Татарстан, р-н Черемшанский, с. Черемшан, 
-ул. Советская, д. 32, пом. 316
+        <v xml:space="preserve">Республика Татарстан, р-н Черемшанский, с. Черемшан, _x000d_
+ул. Советская, д. 32, пом. 316_x000d_
 </v>
       </c>
     </row>
@@ -2508,8 +2508,8 @@
         <v>Акционерное общество «Институт развития организационных структур толивно-энергетического комплекса» (АО «Институт РОСТЭК»)</v>
       </c>
       <c r="C192" t="str" xml:space="preserve">
-        <v xml:space="preserve">край Пермский, город Пермь,
-улица Петропавловская, дом 123, офис 4
+        <v xml:space="preserve">край Пермский, город Пермь,_x000d_
+улица Петропавловская, дом 123, офис 4_x000d_
 </v>
       </c>
     </row>
@@ -2741,7 +2741,7 @@
         <v>ООО «МНКТ»</v>
       </c>
       <c r="C213" t="str" xml:space="preserve">
-        <v xml:space="preserve">Республика Татарстан, город Казань, улица Муштари, дом 2А, пом/офис 100Н/41
+        <v xml:space="preserve">Республика Татарстан, город Казань, улица Муштари, дом 2А, пом/офис 100Н/41_x000d_
 </v>
       </c>
     </row>
@@ -3028,8 +3028,8 @@
         <v>АО «РЕИМПЭКС»</v>
       </c>
       <c r="C239" t="str" xml:space="preserve">
-        <v xml:space="preserve">Самарская область, г. Самара,
-ул. Клиническая, д. 154, литера ИИ2И1, комн.2  
+        <v xml:space="preserve">Самарская область, г. Самара,_x000d_
+ул. Клиническая, д. 154, литера ИИ2И1, комн.2  _x000d_
 </v>
       </c>
     </row>
@@ -3514,7 +3514,7 @@
         <v>АО «Татнефтепром»</v>
       </c>
       <c r="C283" t="str" xml:space="preserve">
-        <v xml:space="preserve">Республика Татарстан, 
+        <v xml:space="preserve">Республика Татарстан, _x000d_
 г. Альметьевск, ул. Маяковского, д. 116</v>
       </c>
     </row>
@@ -3655,8 +3655,8 @@
         <v>144</v>
       </c>
       <c r="B296" t="str" xml:space="preserve">
-        <v xml:space="preserve">Акционерное общество «Томскнефть» Восточной Нефтяной Компании 
-(АО «Томскнефть» ВНК)
+        <v xml:space="preserve">Акционерное общество «Томскнефть» Восточной Нефтяной Компании _x000d_
+(АО «Томскнефть» ВНК)_x000d_
 </v>
       </c>
       <c r="C296" t="str">
@@ -3825,8 +3825,8 @@
         <v>АО «Южно-Аксютино»</v>
       </c>
       <c r="C311" t="str" xml:space="preserve">
-        <v xml:space="preserve">область Московская,
-район Дмитровский, город Дмитров, улица Профессиональная, дом 135, корпус 3, пом. 125
+        <v xml:space="preserve">область Московская,_x000d_
+район Дмитровский, город Дмитров, улица Профессиональная, дом 135, корпус 3, пом. 125_x000d_
 </v>
       </c>
     </row>
@@ -4080,7 +4080,7 @@
         <v>ООО «ИНТЭК-Западная Сибирь»</v>
       </c>
       <c r="C334" t="str" xml:space="preserve">
-        <v xml:space="preserve">Ханты-Мансийский Автономный округ – Югра, город Нижневартовск, улица Мира, дом 24
+        <v xml:space="preserve">Ханты-Мансийский Автономный округ – Югра, город Нижневартовск, улица Мира, дом 24_x000d_
 </v>
       </c>
     </row>
@@ -4540,12 +4540,12 @@
         <v>223</v>
       </c>
       <c r="B376" t="str" xml:space="preserve">
-        <v xml:space="preserve">ООО «ВостокИнвестНефть»
+        <v xml:space="preserve">ООО «ВостокИнвестНефть»_x000d_
 </v>
       </c>
       <c r="C376" t="str" xml:space="preserve">
-        <v xml:space="preserve">Ульяновская область, р.п. Новоспасское, ул. Гагарина, 
-д. 25 
+        <v xml:space="preserve">Ульяновская область, р.п. Новоспасское, ул. Гагарина, _x000d_
+д. 25 _x000d_
 </v>
       </c>
     </row>
@@ -4554,11 +4554,11 @@
         <v>223.1</v>
       </c>
       <c r="B377" t="str" xml:space="preserve">
-        <v xml:space="preserve">ООО «НК «ГНТ»
+        <v xml:space="preserve">ООО «НК «ГНТ»_x000d_
 </v>
       </c>
       <c r="C377" t="str" xml:space="preserve">
-        <v xml:space="preserve">Саратовская область, г. Саратов, ул. Соборная, д. 21М
+        <v xml:space="preserve">Саратовская область, г. Саратов, ул. Соборная, д. 21М_x000d_
 </v>
       </c>
     </row>
@@ -4603,8 +4603,8 @@
         <v>ООО «НЗНП Трейд»</v>
       </c>
       <c r="C381" t="str" xml:space="preserve">
-        <v xml:space="preserve">Тюменская область, г. Тюмень, ул. Республики, 
-д. 143А, оф. 1401
+        <v xml:space="preserve">Тюменская область, г. Тюмень, ул. Республики, _x000d_
+д. 143А, оф. 1401_x000d_
 </v>
       </c>
     </row>
@@ -4635,12 +4635,12 @@
         <v>230</v>
       </c>
       <c r="B384" t="str" xml:space="preserve">
-        <v xml:space="preserve">
-ООО « Преображенское»
+        <v xml:space="preserve">_x000d_
+ООО « Преображенское»_x000d_
 </v>
       </c>
       <c r="C384" t="str" xml:space="preserve">
-        <v xml:space="preserve">Оренбургская область, г. Оренбург, ул. Джангильдина,
+        <v xml:space="preserve">Оренбургская область, г. Оренбург, ул. Джангильдина,_x000d_
 д. 3, пом. 12</v>
       </c>
     </row>
@@ -4649,12 +4649,12 @@
         <v>231</v>
       </c>
       <c r="B385" t="str" xml:space="preserve">
-        <v xml:space="preserve">АО «Нефтегазрезерв»
+        <v xml:space="preserve">АО «Нефтегазрезерв»_x000d_
 </v>
       </c>
       <c r="C385" t="str" xml:space="preserve">
-        <v xml:space="preserve">Саратовская область,  г. Саратов, ул. им. Пугачева Е.И.,
-д. 159, оф. 905А
+        <v xml:space="preserve">Саратовская область,  г. Саратов, ул. им. Пугачева Е.И.,_x000d_
+д. 159, оф. 905А_x000d_
 </v>
       </c>
     </row>
@@ -4663,11 +4663,11 @@
         <v>232</v>
       </c>
       <c r="B386" t="str" xml:space="preserve">
-        <v xml:space="preserve">ООО «Дубровинское»
+        <v xml:space="preserve">ООО «Дубровинское»_x000d_
 </v>
       </c>
       <c r="C386" t="str" xml:space="preserve">
-        <v xml:space="preserve">Удмуртская республика, г. Ижевск, ул. им. Репина, д. 35/1, кв. 106
+        <v xml:space="preserve">Удмуртская республика, г. Ижевск, ул. им. Репина, д. 35/1, кв. 106_x000d_
 </v>
       </c>
     </row>
@@ -4676,12 +4676,12 @@
         <v>233</v>
       </c>
       <c r="B387" t="str" xml:space="preserve">
-        <v xml:space="preserve">ООО «Азинское»
+        <v xml:space="preserve">ООО «Азинское»_x000d_
 </v>
       </c>
       <c r="C387" t="str" xml:space="preserve">
-        <v xml:space="preserve">Удмуртская республика, г. Ижевск, ул. им. Репина, 
-д. 35/1, кв. 106
+        <v xml:space="preserve">Удмуртская республика, г. Ижевск, ул. им. Репина, _x000d_
+д. 35/1, кв. 106_x000d_
 </v>
       </c>
     </row>
@@ -4690,12 +4690,12 @@
         <v>234</v>
       </c>
       <c r="B388" t="str" xml:space="preserve">
-        <v xml:space="preserve">Акционерное общество «Антипинский нефтеперерабатывающий
+        <v xml:space="preserve">Акционерное общество «Антипинский нефтеперерабатывающий_x000d_
  завод» (АО «Антипинский НПЗ»)</v>
       </c>
       <c r="C388" t="str" xml:space="preserve">
-        <v xml:space="preserve">Тюменская область,
-г. Тюмень, ул. 6 км Старого Тобольского тракта, д. 20
+        <v xml:space="preserve">Тюменская область,_x000d_
+г. Тюмень, ул. 6 км Старого Тобольского тракта, д. 20_x000d_
 </v>
       </c>
     </row>
@@ -4704,11 +4704,11 @@
         <v>234.1</v>
       </c>
       <c r="B389" t="str" xml:space="preserve">
-        <v xml:space="preserve">Общество с ограниченной ответственностью «Нефтяная компания «Новый Поток» 
+        <v xml:space="preserve">Общество с ограниченной ответственностью «Нефтяная компания «Новый Поток» _x000d_
 (ООО «НКНП»)</v>
       </c>
       <c r="C389" t="str" xml:space="preserve">
-        <v xml:space="preserve">Оренбургская область, г. Бузулук, ул. Матросова, д. 1
+        <v xml:space="preserve">Оренбургская область, г. Бузулук, ул. Матросова, д. 1_x000d_
 </v>
       </c>
     </row>
@@ -4805,11 +4805,11 @@
         <v>241</v>
       </c>
       <c r="B398" t="str" xml:space="preserve">
-        <v xml:space="preserve">ООО «Артамира»
+        <v xml:space="preserve">ООО «Артамира»_x000d_
 </v>
       </c>
       <c r="C398" t="str" xml:space="preserve">
-        <v xml:space="preserve">Саратовская обл., г. Саратов, ул. Вольская, д. 91
+        <v xml:space="preserve">Саратовская обл., г. Саратов, ул. Вольская, д. 91_x000d_
 </v>
       </c>
     </row>
@@ -4832,7 +4832,7 @@
         <v>ООО «Ольшанское»</v>
       </c>
       <c r="C400" t="str" xml:space="preserve">
-        <v xml:space="preserve">Оренбургская область, г. Оренбург,ул. Джангильдина,
+        <v xml:space="preserve">Оренбургская область, г. Оренбург,ул. Джангильдина,_x000d_
  д. 3, пом. 12</v>
       </c>
     </row>
@@ -4877,7 +4877,7 @@
         <v>ООО «НК «Действие»</v>
       </c>
       <c r="C404" t="str" xml:space="preserve">
-        <v xml:space="preserve">Самарская область, г. Самара, ул. Ново-Садовая, д. 106, 
+        <v xml:space="preserve">Самарская область, г. Самара, ул. Ново-Садовая, д. 106, _x000d_
 корп. 82, оф. 26</v>
       </c>
     </row>
@@ -4889,8 +4889,8 @@
         <v>ООО «Кулигинское»</v>
       </c>
       <c r="C405" t="str" xml:space="preserve">
-        <v xml:space="preserve">Республика Удмуртская, г. Ижевск, ул. им. Репина,
-д. 35/1, кв. 106
+        <v xml:space="preserve">Республика Удмуртская, г. Ижевск, ул. им. Репина,_x000d_
+д. 35/1, кв. 106_x000d_
 </v>
       </c>
     </row>
@@ -4902,8 +4902,8 @@
         <v>ООО «Опаринское»</v>
       </c>
       <c r="C406" t="str" xml:space="preserve">
-        <v xml:space="preserve">Республика Удмуртская, г. Ижевск, ул. им. Репина,
-д. 35/1, кв. 106
+        <v xml:space="preserve">Республика Удмуртская, г. Ижевск, ул. им. Репина,_x000d_
+д. 35/1, кв. 106_x000d_
 </v>
       </c>
     </row>
@@ -4915,7 +4915,7 @@
         <v>ООО «Сладковско-Заречное»</v>
       </c>
       <c r="C407" t="str" xml:space="preserve">
-        <v xml:space="preserve">Оренбургская обл., г. Оренбург, ул. Комсомольская, 
+        <v xml:space="preserve">Оренбургская обл., г. Оренбург, ул. Комсомольская, _x000d_
 д. 40</v>
       </c>
     </row>
@@ -4927,8 +4927,8 @@
         <v>ООО «НК «СОЮЗ-НЕФТЬ»</v>
       </c>
       <c r="C408" t="str" xml:space="preserve">
-        <v xml:space="preserve">Саратовская обл., г. Саратов, ул. им. Пугачева Е.И. , 
-д. 159, оф. 606
+        <v xml:space="preserve">Саратовская обл., г. Саратов, ул. им. Пугачева Е.И. , _x000d_
+д. 159, оф. 606_x000d_
 </v>
       </c>
     </row>
@@ -4951,8 +4951,8 @@
         <v>ООО «Ноябрьское»</v>
       </c>
       <c r="C410" t="str" xml:space="preserve">
-        <v xml:space="preserve">Ямало-Ненецкий автономный округ, г. Ноябрьск, 
-ул. Ленина,д. 51
+        <v xml:space="preserve">Ямало-Ненецкий автономный округ, г. Ноябрьск, _x000d_
+ул. Ленина,д. 51_x000d_
 </v>
       </c>
     </row>
@@ -4964,7 +4964,7 @@
         <v>ООО «Мултановский»</v>
       </c>
       <c r="C411" t="str" xml:space="preserve">
-        <v xml:space="preserve">г. Москва, ул. Профсоюзная, д. 56, каб. 77
+        <v xml:space="preserve">г. Москва, ул. Профсоюзная, д. 56, каб. 77_x000d_
 </v>
       </c>
     </row>

</xml_diff>